<commit_message>
add formula to excel_output_template
</commit_message>
<xml_diff>
--- a/excel_output_template.xlsx
+++ b/excel_output_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhananjay/velocius-ai/orix-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF038647-69C6-8644-8AE8-0084AD5D8685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE991D1-05C0-5C49-BFC5-28DD3266216B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{17EE1EEE-A413-E046-A63C-8B8D4D15933C}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Balance Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="Income Statement" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -400,20 +400,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF569CD6"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -425,6 +418,19 @@
       <b/>
       <sz val="13"/>
       <color rgb="FF569CD6"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF242424"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -449,11 +455,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,271 +796,351 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3932893-1622-2B48-9B42-B831D7B4FCA2}">
-  <dimension ref="A1:A51"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="5"/>
     <col min="3" max="3" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" ht="22" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B8" s="4">
+        <f>SUM(B1:B7)</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="B15" s="4">
+        <f>SUM(B9:B14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="B19" s="4">
+        <f>SUM(B16:B18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="B21" s="4">
+        <f>B20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="B22" s="4">
+        <f>B21+B19+B15+B8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="B33" s="4">
+        <f>SUM(B23:B32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+      <c r="B46" s="4">
+        <f>SUM(B34:B45)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+      <c r="B50" s="4">
+        <f>SUM(B47:B49)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>48</v>
+      </c>
+      <c r="B51" s="4">
+        <f>B50+B46+B33</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1063,364 +1151,574 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C347329-90C2-2347-9345-061F951CC602}">
-  <dimension ref="A1:A69"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="5"/>
     <col min="3" max="3" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B4" s="4">
+        <f>SUM(B1:B3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B7" s="4">
+        <f>SUM(B5:B6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="B10" s="4">
+        <f t="shared" ref="B10" si="0">B4+B7+B8+B9</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="B15" s="4">
+        <f t="shared" ref="B15" si="1">SUM(B11:B14)</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="B16" s="4">
+        <f t="shared" ref="B16" si="2">B10+B15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="B20" s="4">
+        <f t="shared" ref="B20" si="3">SUM(B17:B19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="B23" s="4">
+        <f t="shared" ref="B23" si="4">SUM(B21:B22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="B27" s="4">
+        <f t="shared" ref="B27" si="5">SUM(B24:B26)</f>
+        <v>0</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="B30" s="4">
+        <f t="shared" ref="B30" si="6">SUM(B28:B29)</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="B31" s="4">
+        <f t="shared" ref="B31" si="7">B20+B23+B27+B30</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="B32" s="4">
+        <f t="shared" ref="B32" si="8">B16-B31</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+      <c r="B38" s="4">
+        <f t="shared" ref="B38" si="9">SUM(B33:B37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+      <c r="B42" s="4">
+        <f t="shared" ref="B42" si="10">SUM(B39:B41)</f>
+        <v>0</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+      <c r="B52" s="4">
+        <f t="shared" ref="B52" si="11">B32-B38-B42 -SUM(B43:B51)</f>
+        <v>0</v>
+      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+      <c r="B55" s="4">
+        <f t="shared" ref="B55" si="12">SUM(B53:B54)</f>
+        <v>0</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+    </row>
+    <row r="56" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
+      <c r="B56" s="4">
+        <f t="shared" ref="B56" si="13">SUM(B43:B51)</f>
+        <v>0</v>
+      </c>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
+      <c r="B64" s="4">
+        <f t="shared" ref="B64" si="14">B52+SUM(B55,B56,B57:B63)</f>
+        <v>0</v>
+      </c>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
         <v>117</v>
       </c>
+      <c r="B69" s="4">
+        <f>B64+SUM(B65:B68)</f>
+        <v>0</v>
+      </c>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update excel template and change text color to orange for edited fields in excel
</commit_message>
<xml_diff>
--- a/excel_output_template.xlsx
+++ b/excel_output_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhananjay/velocius-ai/orix-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE991D1-05C0-5C49-BFC5-28DD3266216B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E51D12-8370-F040-B5B3-A448894EF5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{17EE1EEE-A413-E046-A63C-8B8D4D15933C}"/>
   </bookViews>
@@ -455,13 +455,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -799,63 +806,63 @@
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="5"/>
-    <col min="3" max="3" width="50.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="60.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="4"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:3" ht="22" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="5">
         <f>SUM(B1:B7)</f>
         <v>0</v>
       </c>
@@ -865,43 +872,43 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="5">
         <f>SUM(B9:B14)</f>
         <v>0</v>
       </c>
@@ -910,25 +917,25 @@
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="5">
         <f>SUM(B16:B18)</f>
         <v>0</v>
       </c>
@@ -937,13 +944,13 @@
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="5">
         <f>B20</f>
         <v>0</v>
       </c>
@@ -952,7 +959,7 @@
       <c r="A22" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="5">
         <f>B21+B19+B15+B8</f>
         <v>0</v>
       </c>
@@ -961,67 +968,67 @@
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="1"/>
+      <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="4"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="1"/>
+      <c r="B32" s="4"/>
     </row>
     <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="5">
         <f>SUM(B23:B32)</f>
         <v>0</v>
       </c>
@@ -1030,79 +1037,79 @@
       <c r="A34" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="1"/>
+      <c r="B34" s="4"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="1"/>
+      <c r="B35" s="4"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="1"/>
+      <c r="B36" s="4"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="1"/>
+      <c r="B37" s="4"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="1"/>
+      <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="1"/>
+      <c r="B39" s="4"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="1"/>
+      <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="1"/>
+      <c r="B41" s="4"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="1"/>
+      <c r="B42" s="4"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="1"/>
+      <c r="B43" s="4"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B44" s="1"/>
+      <c r="B44" s="4"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="1"/>
+      <c r="B45" s="4"/>
     </row>
     <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46" s="5">
         <f>SUM(B34:B45)</f>
         <v>0</v>
       </c>
@@ -1111,25 +1118,25 @@
       <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="1"/>
+      <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B48" s="1"/>
+      <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="1"/>
+      <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B50" s="5">
         <f>SUM(B47:B49)</f>
         <v>0</v>
       </c>
@@ -1138,7 +1145,7 @@
       <c r="A51" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="4">
+      <c r="B51" s="5">
         <f>B50+B46+B33</f>
         <v>0</v>
       </c>
@@ -1155,39 +1162,39 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C4" sqref="C4"/>
+      <selection pane="topRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="5"/>
-    <col min="3" max="3" width="50.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="60.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="5">
         <f>SUM(B1:B3)</f>
         <v>0</v>
       </c>
@@ -1196,19 +1203,19 @@
       <c r="A5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="5">
         <f>SUM(B5:B6)</f>
         <v>0</v>
       </c>
@@ -1217,19 +1224,19 @@
       <c r="A8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="5">
         <f t="shared" ref="B10" si="0">B4+B7+B8+B9</f>
         <v>0</v>
       </c>
@@ -1245,31 +1252,31 @@
       <c r="A11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="5">
         <f t="shared" ref="B15" si="1">SUM(B11:B14)</f>
         <v>0</v>
       </c>
@@ -1285,7 +1292,7 @@
       <c r="A16" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="5">
         <f t="shared" ref="B16" si="2">B10+B15</f>
         <v>0</v>
       </c>
@@ -1294,25 +1301,25 @@
       <c r="A17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="5">
         <f t="shared" ref="B20" si="3">SUM(B17:B19)</f>
         <v>0</v>
       </c>
@@ -1321,19 +1328,19 @@
       <c r="A21" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="5">
         <f t="shared" ref="B23" si="4">SUM(B21:B22)</f>
         <v>0</v>
       </c>
@@ -1342,25 +1349,25 @@
       <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="5">
         <f t="shared" ref="B27" si="5">SUM(B24:B26)</f>
         <v>0</v>
       </c>
@@ -1376,19 +1383,19 @@
       <c r="A28" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="1"/>
+      <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="5">
         <f t="shared" ref="B30" si="6">SUM(B28:B29)</f>
         <v>0</v>
       </c>
@@ -1404,7 +1411,7 @@
       <c r="A31" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="5">
         <f t="shared" ref="B31" si="7">B20+B23+B27+B30</f>
         <v>0</v>
       </c>
@@ -1420,7 +1427,7 @@
       <c r="A32" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="5">
         <f t="shared" ref="B32" si="8">B16-B31</f>
         <v>0</v>
       </c>
@@ -1436,37 +1443,37 @@
       <c r="A33" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="1"/>
+      <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B34" s="1"/>
+      <c r="B34" s="4"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B35" s="1"/>
+      <c r="B35" s="4"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="1"/>
+      <c r="B36" s="4"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="1"/>
+      <c r="B37" s="4"/>
     </row>
     <row r="38" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="5">
         <f t="shared" ref="B38" si="9">SUM(B33:B37)</f>
         <v>0</v>
       </c>
@@ -1475,25 +1482,25 @@
       <c r="A39" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="1"/>
+      <c r="B39" s="4"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="1"/>
+      <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="1"/>
+      <c r="B41" s="4"/>
     </row>
     <row r="42" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="5">
         <f t="shared" ref="B42" si="10">SUM(B39:B41)</f>
         <v>0</v>
       </c>
@@ -1509,61 +1516,61 @@
       <c r="A43" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="1"/>
+      <c r="B43" s="4"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B44" s="1"/>
+      <c r="B44" s="4"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="1"/>
+      <c r="B45" s="4"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B46" s="1"/>
+      <c r="B46" s="4"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="1"/>
+      <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B48" s="1"/>
+      <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="1"/>
+      <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B50" s="1"/>
+      <c r="B50" s="4"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B51" s="1"/>
+      <c r="B51" s="4"/>
     </row>
     <row r="52" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B52" s="4">
+      <c r="B52" s="5">
         <f t="shared" ref="B52" si="11">B32-B38-B42 -SUM(B43:B51)</f>
         <v>0</v>
       </c>
@@ -1579,19 +1586,19 @@
       <c r="A53" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B53" s="1"/>
+      <c r="B53" s="4"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B54" s="1"/>
+      <c r="B54" s="4"/>
     </row>
     <row r="55" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B55" s="4">
+      <c r="B55" s="5">
         <f t="shared" ref="B55" si="12">SUM(B53:B54)</f>
         <v>0</v>
       </c>
@@ -1607,7 +1614,7 @@
       <c r="A56" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B56" s="4">
+      <c r="B56" s="5">
         <f t="shared" ref="B56" si="13">SUM(B43:B51)</f>
         <v>0</v>
       </c>
@@ -1623,49 +1630,49 @@
       <c r="A57" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B57" s="1"/>
+      <c r="B57" s="4"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B58" s="1"/>
+      <c r="B58" s="4"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B59" s="1"/>
+      <c r="B59" s="4"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B60" s="1"/>
+      <c r="B60" s="4"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B61" s="1"/>
+      <c r="B61" s="4"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B62" s="1"/>
+      <c r="B62" s="4"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B63" s="1"/>
+      <c r="B63" s="4"/>
     </row>
     <row r="64" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B64" s="4">
+      <c r="B64" s="5">
         <f t="shared" ref="B64" si="14">B52+SUM(B55,B56,B57:B63)</f>
         <v>0</v>
       </c>
@@ -1681,31 +1688,31 @@
       <c r="A65" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B65" s="1"/>
+      <c r="B65" s="4"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B66" s="1"/>
+      <c r="B66" s="4"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B67" s="1"/>
+      <c r="B67" s="4"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B68" s="1"/>
+      <c r="B68" s="4"/>
     </row>
     <row r="69" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B69" s="5">
         <f>B64+SUM(B65:B68)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
fix inconsistent value UI vs excel issue
</commit_message>
<xml_diff>
--- a/excel_output_template.xlsx
+++ b/excel_output_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhananjay/velocius-ai/orix-poc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhana\projects\orix\orix-poc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E51D12-8370-F040-B5B3-A448894EF5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95F3D4C-1835-47D1-8F9B-D764C6A96555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{17EE1EEE-A413-E046-A63C-8B8D4D15933C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{17EE1EEE-A413-E046-A63C-8B8D4D15933C}"/>
   </bookViews>
   <sheets>
     <sheet name="Balance Sheet" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>Cash</t>
   </si>
@@ -48,9 +46,6 @@
     <t>Accounts Receivable Other</t>
   </si>
   <si>
-    <t>Tenant Security Deposits</t>
-  </si>
-  <si>
     <t>Prepaid Property Insurances</t>
   </si>
   <si>
@@ -394,6 +389,12 @@
   </si>
   <si>
     <t>Miscellaneous Revenue</t>
+  </si>
+  <si>
+    <t>Tenant Security Deposits - Assets</t>
+  </si>
+  <si>
+    <t>Tenant Security Deposits - Liabilities</t>
   </si>
 </sst>
 </file>
@@ -805,62 +806,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3932893-1622-2B48-9B42-B831D7B4FCA2}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="60.83203125" customWidth="1"/>
+    <col min="1" max="1" width="50.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.796875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="60.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="5">
         <f>SUM(B1:B7)</f>
@@ -868,282 +869,282 @@
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="5">
         <f>SUM(B9:B14)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="5">
         <f>SUM(B16:B18)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" s="5">
         <f>B20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22" s="5">
         <f>B21+B19+B15+B8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="4"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" s="4"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="4"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="4"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="4"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="B28" s="4"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="4"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="B29" s="4"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="4"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="B30" s="4"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="4"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="B31" s="4"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="4"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" s="5">
         <f>SUM(B23:B32)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="4"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="4"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="B35" s="4"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="4"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="B36" s="4"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="4"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+      <c r="B37" s="4"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="4"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="B38" s="4"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="4"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="B39" s="4"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="4"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="B40" s="4"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="4"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="B41" s="4"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="4"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="B42" s="4"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="4"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="B43" s="4"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="4"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="B44" s="4"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B44" s="4"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="B45" s="4"/>
     </row>
-    <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" s="5">
         <f>SUM(B34:B45)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B47" s="4"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" s="4"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B48" s="4"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="B49" s="4"/>
     </row>
-    <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B50" s="5">
         <f>SUM(B47:B49)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B51" s="5">
         <f>B50+B46+B33</f>
@@ -1160,81 +1161,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C347329-90C2-2347-9345-061F951CC602}">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="60.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.796875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="60.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" s="5">
         <f>SUM(B1:B3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" s="5">
         <f>SUM(B5:B6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" s="5">
         <f t="shared" ref="B10" si="0">B4+B7+B8+B9</f>
@@ -1248,33 +1249,33 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B15" s="5">
         <f t="shared" ref="B15" si="1">SUM(B11:B14)</f>
@@ -1288,84 +1289,84 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B16" s="5">
         <f t="shared" ref="B16" si="2">B10+B15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B20" s="5">
         <f t="shared" ref="B20" si="3">SUM(B17:B19)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="4"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B23" s="5">
         <f t="shared" ref="B23" si="4">SUM(B21:B22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="4"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="4"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B27" s="5">
         <f t="shared" ref="B27" si="5">SUM(B24:B26)</f>
@@ -1379,21 +1380,21 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="4"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B30" s="5">
         <f t="shared" ref="B30" si="6">SUM(B28:B29)</f>
@@ -1407,9 +1408,9 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B31" s="5">
         <f t="shared" ref="B31" si="7">B20+B23+B27+B30</f>
@@ -1423,9 +1424,9 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B32" s="5">
         <f t="shared" ref="B32" si="8">B16-B31</f>
@@ -1439,66 +1440,66 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="4"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="B34" s="4"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B34" s="4"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="B35" s="4"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B35" s="4"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="B36" s="4"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="4"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B38" s="5">
         <f t="shared" ref="B38" si="9">SUM(B33:B37)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="4"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="B40" s="4"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="4"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B42" s="5">
         <f t="shared" ref="B42" si="10">SUM(B39:B41)</f>
@@ -1512,63 +1513,63 @@
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="4"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="B44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B44" s="4"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="B45" s="4"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="4"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="B46" s="4"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B46" s="4"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+      <c r="B47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="4"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="B48" s="4"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B48" s="4"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+      <c r="B49" s="4"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="4"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+      <c r="B50" s="4"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B50" s="4"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="B51" s="4"/>
     </row>
-    <row r="52" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B52" s="5">
         <f t="shared" ref="B52" si="11">B32-B38-B42 -SUM(B43:B51)</f>
@@ -1582,21 +1583,21 @@
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53" s="4"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B53" s="4"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="B54" s="4"/>
     </row>
-    <row r="55" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B55" s="5">
         <f t="shared" ref="B55" si="12">SUM(B53:B54)</f>
@@ -1610,9 +1611,9 @@
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
     </row>
-    <row r="56" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B56" s="5">
         <f t="shared" ref="B56" si="13">SUM(B43:B51)</f>
@@ -1626,51 +1627,51 @@
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" s="4"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B57" s="4"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+      <c r="B58" s="4"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B58" s="4"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+      <c r="B59" s="4"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B59" s="4"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+      <c r="B60" s="4"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B60" s="4"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+      <c r="B61" s="4"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B61" s="4"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+      <c r="B62" s="4"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B62" s="4"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="B63" s="4"/>
     </row>
-    <row r="64" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B64" s="5">
         <f t="shared" ref="B64" si="14">B52+SUM(B55,B56,B57:B63)</f>
@@ -1684,33 +1685,33 @@
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B65" s="4"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B65" s="4"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+      <c r="B66" s="4"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B66" s="4"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
+      <c r="B67" s="4"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B67" s="4"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="B68" s="4"/>
     </row>
-    <row r="69" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B69" s="5">
         <f>B64+SUM(B65:B68)</f>

</xml_diff>

<commit_message>
Revert "Add User feedback feature to DEV"
</commit_message>
<xml_diff>
--- a/excel_output_template.xlsx
+++ b/excel_output_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhana\projects\orix\orix-poc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhananjay/velocius-ai/orix-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95F3D4C-1835-47D1-8F9B-D764C6A96555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E51D12-8370-F040-B5B3-A448894EF5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{17EE1EEE-A413-E046-A63C-8B8D4D15933C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{17EE1EEE-A413-E046-A63C-8B8D4D15933C}"/>
   </bookViews>
   <sheets>
     <sheet name="Balance Sheet" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="119">
   <si>
     <t>Cash</t>
   </si>
@@ -46,6 +48,9 @@
     <t>Accounts Receivable Other</t>
   </si>
   <si>
+    <t>Tenant Security Deposits</t>
+  </si>
+  <si>
     <t>Prepaid Property Insurances</t>
   </si>
   <si>
@@ -389,12 +394,6 @@
   </si>
   <si>
     <t>Miscellaneous Revenue</t>
-  </si>
-  <si>
-    <t>Tenant Security Deposits - Assets</t>
-  </si>
-  <si>
-    <t>Tenant Security Deposits - Liabilities</t>
   </si>
 </sst>
 </file>
@@ -806,62 +805,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3932893-1622-2B48-9B42-B831D7B4FCA2}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.796875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="60.796875" customWidth="1"/>
+    <col min="1" max="1" width="50.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="60.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>118</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="22" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" s="5">
         <f>SUM(B1:B7)</f>
@@ -869,282 +868,282 @@
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" s="5">
         <f>SUM(B9:B14)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B19" s="5">
         <f>SUM(B16:B18)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B21" s="5">
         <f>B20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B22" s="5">
         <f>B21+B19+B15+B8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>119</v>
+        <v>3</v>
       </c>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B33" s="5">
         <f>SUM(B23:B32)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B38" s="4"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B42" s="4"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B43" s="4"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B44" s="4"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B45" s="4"/>
     </row>
-    <row r="46" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" s="5">
         <f>SUM(B34:B45)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B47" s="4"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B48" s="4"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B49" s="4"/>
     </row>
-    <row r="50" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B50" s="5">
         <f>SUM(B47:B49)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B51" s="5">
         <f>B50+B46+B33</f>
@@ -1161,81 +1160,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C347329-90C2-2347-9345-061F951CC602}">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.796875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="60.796875" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="60.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B4" s="5">
         <f>SUM(B1:B3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B7" s="5">
         <f>SUM(B5:B6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B10" s="5">
         <f t="shared" ref="B10" si="0">B4+B7+B8+B9</f>
@@ -1249,33 +1248,33 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B15" s="5">
         <f t="shared" ref="B15" si="1">SUM(B11:B14)</f>
@@ -1289,84 +1288,84 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B16" s="5">
         <f t="shared" ref="B16" si="2">B10+B15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B20" s="5">
         <f t="shared" ref="B20" si="3">SUM(B17:B19)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B23" s="5">
         <f t="shared" ref="B23" si="4">SUM(B21:B22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B27" s="5">
         <f t="shared" ref="B27" si="5">SUM(B24:B26)</f>
@@ -1380,21 +1379,21 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B30" s="5">
         <f t="shared" ref="B30" si="6">SUM(B28:B29)</f>
@@ -1408,9 +1407,9 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B31" s="5">
         <f t="shared" ref="B31" si="7">B20+B23+B27+B30</f>
@@ -1424,9 +1423,9 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B32" s="5">
         <f t="shared" ref="B32" si="8">B16-B31</f>
@@ -1440,66 +1439,66 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B38" s="5">
         <f t="shared" ref="B38" si="9">SUM(B33:B37)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B42" s="5">
         <f t="shared" ref="B42" si="10">SUM(B39:B41)</f>
@@ -1513,63 +1512,63 @@
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B43" s="4"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B44" s="4"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B45" s="4"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B46" s="4"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B47" s="4"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B48" s="4"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B49" s="4"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B50" s="4"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B51" s="4"/>
     </row>
-    <row r="52" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B52" s="5">
         <f t="shared" ref="B52" si="11">B32-B38-B42 -SUM(B43:B51)</f>
@@ -1583,21 +1582,21 @@
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B53" s="4"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B54" s="4"/>
     </row>
-    <row r="55" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B55" s="5">
         <f t="shared" ref="B55" si="12">SUM(B53:B54)</f>
@@ -1611,9 +1610,9 @@
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
     </row>
-    <row r="56" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B56" s="5">
         <f t="shared" ref="B56" si="13">SUM(B43:B51)</f>
@@ -1627,51 +1626,51 @@
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B57" s="4"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B58" s="4"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B59" s="4"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B60" s="4"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B61" s="4"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B62" s="4"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B63" s="4"/>
     </row>
-    <row r="64" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B64" s="5">
         <f t="shared" ref="B64" si="14">B52+SUM(B55,B56,B57:B63)</f>
@@ -1685,33 +1684,33 @@
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B65" s="4"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B66" s="4"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B67" s="4"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B68" s="4"/>
     </row>
-    <row r="69" spans="1:9" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B69" s="5">
         <f>B64+SUM(B65:B68)</f>

</xml_diff>